<commit_message>
LIS pilot feedback update * Narrowed conditions to just 2 choices: OK, BAD * Switch ID from Lab ID to STT ID on result forms * Updated the STT ID label
</commit_message>
<xml_diff>
--- a/rarrive.xlsx
+++ b/rarrive.xlsx
@@ -93,10 +93,10 @@
     <t>barcode</t>
   </si>
   <si>
-    <t>labid</t>
-  </si>
-  <si>
-    <t>Lab Barcode</t>
+    <t>stid</t>
+  </si>
+  <si>
+    <t>STT Barcode</t>
   </si>
   <si>
     <t>end repeat</t>
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -228,6 +228,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -392,10 +395,10 @@
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -442,29 +445,29 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
@@ -524,7 +527,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -539,18 +542,18 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>